<commit_message>
Add all widgets back
</commit_message>
<xml_diff>
--- a/public/accidents-excel/Rijkswaterstaat-accidents.xlsx
+++ b/public/accidents-excel/Rijkswaterstaat-accidents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elidu/Repos/widget-demos/public/accidents-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CF090C1-5972-7A4B-807B-B4FF73C72AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C998B695-76E9-3B47-9C77-8D50F1F6EEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19660" xr2:uid="{2AE93F08-5D1B-CF4C-9ADA-D1635E2263DF}"/>
   </bookViews>
@@ -3970,8 +3970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF114F92-FA8C-2C46-8C4F-5C9E3C0F5093}">
   <dimension ref="A1:BK510"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
+      <selection activeCell="B286" sqref="B286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3981,13 +3981,14 @@
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.83203125" customWidth="1"/>
+    <col min="13" max="13" width="40.1640625" customWidth="1"/>
     <col min="14" max="14" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.5" bestFit="1" customWidth="1"/>

</xml_diff>